<commit_message>
Update version number in main.ts, add exportToExcel endpoint in stocks.controller.ts, and add exportToExcel method in stocks.service.ts
</commit_message>
<xml_diff>
--- a/templates/StokListesi.xlsx
+++ b/templates/StokListesi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALİ RIZA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ersaa\vip-pos-v0.1\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A60BF03-F62F-40B0-8C35-86D5BCF7A553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C7FFE6-7BBE-4652-B5B4-D20511516D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,39 +480,39 @@
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC19" sqref="AC19"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="9" width="10.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
-    <col min="11" max="14" width="14.85546875" style="1" customWidth="1"/>
+    <col min="5" max="9" width="10.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="11" max="14" width="14.88671875" style="1" customWidth="1"/>
     <col min="15" max="15" width="17" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="16" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="17" style="1" customWidth="1"/>
     <col min="20" max="20" width="16" style="1" customWidth="1"/>
-    <col min="21" max="21" width="22.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="21.5703125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" style="1" customWidth="1"/>
-    <col min="26" max="29" width="13.85546875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.85546875" style="2" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="10.28515625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="22.5546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.44140625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" style="1" customWidth="1"/>
+    <col min="26" max="29" width="13.88671875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.88671875" style="2" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" style="2" customWidth="1"/>
+    <col min="32" max="32" width="10.33203125" style="2" customWidth="1"/>
     <col min="33" max="33" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +613,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -717,6 +717,6 @@
   </sheetData>
   <autoFilter ref="A1:AG2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToWidth="0" fitToHeight="0"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>